<commit_message>
update ngày hôm qua
</commit_message>
<xml_diff>
--- a/WebNewBook/File/file_mau.xlsx
+++ b/WebNewBook/File/file_mau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Le Cuong\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C4E9E6-A402-4A6B-AE5B-8E84C23488F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7AD779-BFED-4E16-889F-D9F7B3CF520B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1463" windowWidth="14400" windowHeight="7387" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File" sheetId="2" r:id="rId1"/>
@@ -20,18 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Mã Voucher</t>
   </si>
   <si>
-    <t>KTC7</t>
-  </si>
-  <si>
-    <t>KTC8</t>
-  </si>
-  <si>
-    <t>KTC9</t>
+    <t>TANG-PHONG-1</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-2</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-3</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-4</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-5</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-6</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-7</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-8</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-9</t>
+  </si>
+  <si>
+    <t>TANG-PHONG-10</t>
   </si>
 </sst>
 </file>
@@ -375,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -403,6 +424,41 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>